<commit_message>
updating Excel sheets to make consistent
</commit_message>
<xml_diff>
--- a/Preventive Care Screening MedStart.xlsx
+++ b/Preventive Care Screening MedStart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
+    <workbookView xWindow="3960" yWindow="660" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="195">
   <si>
     <t>Indications</t>
   </si>
@@ -75,9 +75,6 @@
     <t>glucocorticoid therapy</t>
   </si>
   <si>
-    <t>parental hip fracture</t>
-  </si>
-  <si>
     <t>parental Hx of hip fracture</t>
   </si>
   <si>
@@ -153,9 +150,6 @@
     <t>Birthplace: Africa</t>
   </si>
   <si>
-    <t>Birthplace: Asia</t>
-  </si>
-  <si>
     <t>30 pack year smoking history</t>
   </si>
   <si>
@@ -327,9 +321,6 @@
     <t>ckFFatherBrotherProsCancer</t>
   </si>
   <si>
-    <t>ckBBirthLoc</t>
-  </si>
-  <si>
     <t>ckPCOPD</t>
   </si>
   <si>
@@ -592,6 +583,27 @@
   </si>
   <si>
     <t>Offer Hep B vaccine</t>
+  </si>
+  <si>
+    <t>ckSexuallyActive</t>
+  </si>
+  <si>
+    <t>ckEarlyMenopause</t>
+  </si>
+  <si>
+    <t>ckChronicLiverDisease</t>
+  </si>
+  <si>
+    <t>ckBBirthAfAs</t>
+  </si>
+  <si>
+    <t>ckEndStageRenal</t>
+  </si>
+  <si>
+    <t>ckInjectionDrug</t>
+  </si>
+  <si>
+    <t>ckNegativeHPV</t>
   </si>
 </sst>
 </file>
@@ -658,8 +670,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -699,7 +723,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -709,6 +733,12 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -718,6 +748,12 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1047,19 +1083,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BZ147"/>
+  <dimension ref="A1:BW147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:BZ1048576"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="AD37" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="AJ46" sqref="AJ46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="78" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" customWidth="1"/>
+    <col min="3" max="75" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" ht="12.75" customHeight="1">
+    <row r="1" spans="1:75" ht="12.75" customHeight="1">
       <c r="B1" s="4"/>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -1067,10 +1106,10 @@
       <c r="J1" t="s">
         <v>1</v>
       </c>
-      <c r="V1" s="4"/>
-      <c r="Z1" s="4"/>
-    </row>
-    <row r="2" spans="1:78" ht="12.75" customHeight="1">
+      <c r="T1" s="4"/>
+      <c r="X1" s="4"/>
+    </row>
+    <row r="2" spans="1:75" ht="12.75" customHeight="1">
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1123,270 +1162,279 @@
         <v>18</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AF2" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AH2" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AI2" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AJ2" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AK2" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AL2" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AM2" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AN2" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AO2" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AP2" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AQ2" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AR2" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AS2" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AT2" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AU2" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AV2" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AW2" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AX2" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AY2" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AZ2" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="BA2" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="BB2" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="BC2" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="BD2" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="BE2" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="BF2" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="BG2" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="BH2" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BI2" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="BJ2" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="BK2" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="BL2" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="BM2" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="BN2" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="BO2" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="BP2" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="BQ2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="BR2" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="BS2" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="BT2" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="BU2" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="BV2" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="BW2" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="BX2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BY2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:75" ht="12.75" customHeight="1">
+      <c r="A3" t="s">
         <v>76</v>
-      </c>
-      <c r="BZ2" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:78" ht="12.75" customHeight="1">
-      <c r="A3" t="s">
-        <v>78</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
       </c>
+      <c r="F3" t="s">
+        <v>188</v>
+      </c>
       <c r="G3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" t="s">
         <v>79</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>80</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>81</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>82</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>83</v>
       </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
         <v>84</v>
       </c>
-      <c r="M3" t="s">
+      <c r="O3" t="s">
         <v>85</v>
       </c>
-      <c r="N3" t="s">
+      <c r="P3" t="s">
         <v>86</v>
       </c>
-      <c r="O3" t="s">
+      <c r="Q3" t="s">
         <v>87</v>
       </c>
-      <c r="P3" t="s">
+      <c r="R3" t="s">
         <v>88</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="T3" t="s">
         <v>89</v>
       </c>
-      <c r="T3" t="s">
+      <c r="V3" t="s">
         <v>90</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>91</v>
       </c>
       <c r="X3" t="s">
+        <v>189</v>
+      </c>
+      <c r="Y3" t="s">
         <v>92</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>93</v>
       </c>
       <c r="AA3" t="s">
+        <v>190</v>
+      </c>
+      <c r="AB3" t="s">
         <v>94</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AF3" t="s">
         <v>95</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AH3" t="s">
+        <v>194</v>
+      </c>
+      <c r="AJ3" t="s">
         <v>96</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AL3" t="s">
         <v>97</v>
       </c>
-      <c r="AL3" t="s">
+      <c r="AN3" t="s">
         <v>98</v>
       </c>
-      <c r="AN3" t="s">
+      <c r="AO3" t="s">
         <v>99</v>
       </c>
       <c r="AP3" t="s">
+        <v>191</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AY3" t="s">
         <v>100</v>
       </c>
-      <c r="AQ3" t="s">
+      <c r="AZ3" t="s">
         <v>101</v>
       </c>
-      <c r="AR3" t="s">
+      <c r="BA3" t="s">
         <v>102</v>
-      </c>
-      <c r="AS3" t="s">
-        <v>102</v>
-      </c>
-      <c r="AW3" t="s">
-        <v>79</v>
       </c>
       <c r="BB3" t="s">
         <v>103</v>
@@ -1400,13 +1448,13 @@
       <c r="BE3" t="s">
         <v>106</v>
       </c>
-      <c r="BF3" t="s">
+      <c r="BG3" t="s">
         <v>107</v>
       </c>
-      <c r="BG3" t="s">
+      <c r="BH3" t="s">
         <v>108</v>
       </c>
-      <c r="BH3" t="s">
+      <c r="BI3" t="s">
         <v>109</v>
       </c>
       <c r="BJ3" t="s">
@@ -1427,37 +1475,34 @@
       <c r="BO3" t="s">
         <v>115</v>
       </c>
-      <c r="BP3" t="s">
+      <c r="BQ3" t="s">
         <v>116</v>
       </c>
-      <c r="BQ3" t="s">
+      <c r="BR3" t="s">
         <v>117</v>
       </c>
-      <c r="BR3" t="s">
+      <c r="BS3" t="s">
         <v>118</v>
       </c>
       <c r="BT3" t="s">
         <v>119</v>
       </c>
       <c r="BU3" t="s">
+        <v>193</v>
+      </c>
+      <c r="BV3" t="s">
         <v>120</v>
       </c>
-      <c r="BV3" t="s">
+      <c r="BW3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="1:75" ht="12.75" customHeight="1">
+      <c r="A4" t="s">
         <v>121</v>
       </c>
-      <c r="BW3" t="s">
+      <c r="B4" t="s">
         <v>122</v>
-      </c>
-      <c r="BY3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4" spans="1:78" ht="12.75" customHeight="1">
-      <c r="A4" t="s">
-        <v>124</v>
-      </c>
-      <c r="B4" t="s">
-        <v>125</v>
       </c>
       <c r="C4">
         <v>24</v>
@@ -1466,417 +1511,411 @@
         <v>24</v>
       </c>
       <c r="E4" t="s">
+        <v>123</v>
+      </c>
+      <c r="F4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:75" ht="12.75" customHeight="1">
+      <c r="A5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" t="s">
+        <v>122</v>
+      </c>
+      <c r="G5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:75" ht="12.75" customHeight="1">
+      <c r="A7" t="s">
         <v>126</v>
       </c>
-      <c r="F4" t="s">
+      <c r="B7" t="s">
         <v>127</v>
-      </c>
-    </row>
-    <row r="5" spans="1:78" ht="12.75" customHeight="1">
-      <c r="A5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B5" t="s">
-        <v>125</v>
-      </c>
-      <c r="G5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="7" spans="1:78" ht="12.75" customHeight="1">
-      <c r="A7" t="s">
-        <v>129</v>
-      </c>
-      <c r="B7" t="s">
-        <v>130</v>
       </c>
       <c r="D7">
         <v>24</v>
       </c>
       <c r="E7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:75" ht="12.75" customHeight="1">
+      <c r="A8" t="s">
         <v>126</v>
       </c>
-      <c r="F7" t="s">
+      <c r="B8" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="8" spans="1:78" ht="12.75" customHeight="1">
-      <c r="A8" t="s">
+      <c r="G8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:75" ht="12.75" customHeight="1">
+      <c r="A10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B10" t="s">
         <v>129</v>
       </c>
-      <c r="B8" t="s">
+      <c r="E10" t="s">
         <v>130</v>
       </c>
-      <c r="G8" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="10" spans="1:78" ht="12.75" customHeight="1">
-      <c r="A10" t="s">
+      <c r="F10" t="s">
+        <v>124</v>
+      </c>
+      <c r="G10" t="s">
+        <v>124</v>
+      </c>
+      <c r="H10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:75" ht="12.75" customHeight="1">
+      <c r="B12" t="s">
         <v>131</v>
-      </c>
-      <c r="B10" t="s">
-        <v>132</v>
-      </c>
-      <c r="E10" t="s">
-        <v>133</v>
-      </c>
-      <c r="F10" t="s">
-        <v>127</v>
-      </c>
-      <c r="G10" t="s">
-        <v>127</v>
-      </c>
-      <c r="H10" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="12" spans="1:78" ht="12.75" customHeight="1">
-      <c r="B12" t="s">
-        <v>134</v>
       </c>
       <c r="C12">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:78" ht="12.75" customHeight="1">
+    <row r="13" spans="1:75" ht="12.75" customHeight="1">
       <c r="B13" t="s">
+        <v>131</v>
+      </c>
+      <c r="I13" t="s">
+        <v>132</v>
+      </c>
+      <c r="J13" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:75" ht="12.75" customHeight="1">
+      <c r="B14" t="s">
+        <v>131</v>
+      </c>
+      <c r="I14" t="s">
+        <v>132</v>
+      </c>
+      <c r="K14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:75" ht="12.75" customHeight="1">
+      <c r="B15" t="s">
+        <v>131</v>
+      </c>
+      <c r="I15" t="s">
+        <v>132</v>
+      </c>
+      <c r="L15" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="1:75" ht="12.75" customHeight="1">
+      <c r="B16" t="s">
+        <v>131</v>
+      </c>
+      <c r="I16" t="s">
+        <v>132</v>
+      </c>
+      <c r="M16" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" ht="12.75" customHeight="1">
+      <c r="B17" t="s">
+        <v>131</v>
+      </c>
+      <c r="I17" t="s">
+        <v>132</v>
+      </c>
+      <c r="N17" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" ht="12.75" customHeight="1">
+      <c r="A19" t="s">
+        <v>133</v>
+      </c>
+      <c r="B19" t="s">
         <v>134</v>
-      </c>
-      <c r="I13" t="s">
-        <v>135</v>
-      </c>
-      <c r="J13" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="14" spans="1:78" ht="12.75" customHeight="1">
-      <c r="B14" t="s">
-        <v>134</v>
-      </c>
-      <c r="I14" t="s">
-        <v>135</v>
-      </c>
-      <c r="K14" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="15" spans="1:78" ht="12.75" customHeight="1">
-      <c r="B15" t="s">
-        <v>134</v>
-      </c>
-      <c r="I15" t="s">
-        <v>135</v>
-      </c>
-      <c r="L15" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="16" spans="1:78" ht="12.75" customHeight="1">
-      <c r="B16" t="s">
-        <v>134</v>
-      </c>
-      <c r="I16" t="s">
-        <v>135</v>
-      </c>
-      <c r="M16" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="17" spans="1:28" ht="12.75" customHeight="1">
-      <c r="B17" t="s">
-        <v>134</v>
-      </c>
-      <c r="I17" t="s">
-        <v>135</v>
-      </c>
-      <c r="N17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="19" spans="1:28" ht="12.75" customHeight="1">
-      <c r="A19" t="s">
-        <v>136</v>
-      </c>
-      <c r="B19" t="s">
-        <v>137</v>
       </c>
       <c r="C19">
         <v>65</v>
       </c>
       <c r="E19" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="20" spans="1:28" ht="12.75" customHeight="1">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" ht="12.75" customHeight="1">
       <c r="A20" t="s">
+        <v>133</v>
+      </c>
+      <c r="B20" t="s">
+        <v>135</v>
+      </c>
+      <c r="E20" t="s">
+        <v>123</v>
+      </c>
+      <c r="O20" t="s">
+        <v>124</v>
+      </c>
+      <c r="P20" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" ht="12.75" customHeight="1">
+      <c r="A21" t="s">
+        <v>133</v>
+      </c>
+      <c r="B21" t="s">
+        <v>135</v>
+      </c>
+      <c r="E21" t="s">
+        <v>123</v>
+      </c>
+      <c r="O21" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" ht="12.75" customHeight="1">
+      <c r="A22" t="s">
+        <v>133</v>
+      </c>
+      <c r="B22" t="s">
+        <v>135</v>
+      </c>
+      <c r="E22" t="s">
+        <v>123</v>
+      </c>
+      <c r="O22" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" ht="12.75" customHeight="1">
+      <c r="A23" t="s">
+        <v>133</v>
+      </c>
+      <c r="B23" t="s">
+        <v>135</v>
+      </c>
+      <c r="E23" t="s">
+        <v>123</v>
+      </c>
+      <c r="O23" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" ht="12.75" customHeight="1">
+      <c r="A24" t="s">
+        <v>133</v>
+      </c>
+      <c r="B24" t="s">
+        <v>135</v>
+      </c>
+      <c r="E24" t="s">
+        <v>123</v>
+      </c>
+      <c r="O24" t="s">
+        <v>124</v>
+      </c>
+      <c r="R24" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" ht="12.75" customHeight="1">
+      <c r="A25" t="s">
+        <v>133</v>
+      </c>
+      <c r="B25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E25" t="s">
+        <v>123</v>
+      </c>
+      <c r="O25" t="s">
+        <v>124</v>
+      </c>
+      <c r="S25" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" ht="12.75" customHeight="1">
+      <c r="A26" t="s">
+        <v>133</v>
+      </c>
+      <c r="B26" t="s">
+        <v>135</v>
+      </c>
+      <c r="E26" t="s">
+        <v>123</v>
+      </c>
+      <c r="O26" t="s">
+        <v>124</v>
+      </c>
+      <c r="T26" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" ht="12.75" customHeight="1">
+      <c r="A27" t="s">
+        <v>133</v>
+      </c>
+      <c r="B27" t="s">
+        <v>135</v>
+      </c>
+      <c r="E27" t="s">
+        <v>123</v>
+      </c>
+      <c r="O27" t="s">
+        <v>124</v>
+      </c>
+      <c r="U27" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" ht="12.75" customHeight="1">
+      <c r="A28" t="s">
+        <v>133</v>
+      </c>
+      <c r="B28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E28" t="s">
+        <v>123</v>
+      </c>
+      <c r="O28" t="s">
+        <v>124</v>
+      </c>
+      <c r="V28" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" ht="12.75" customHeight="1">
+      <c r="A29" t="s">
+        <v>133</v>
+      </c>
+      <c r="B29" t="s">
+        <v>135</v>
+      </c>
+      <c r="E29" t="s">
+        <v>123</v>
+      </c>
+      <c r="O29" t="s">
+        <v>124</v>
+      </c>
+      <c r="W29" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" ht="12.75" customHeight="1">
+      <c r="A30" t="s">
+        <v>133</v>
+      </c>
+      <c r="B30" t="s">
+        <v>135</v>
+      </c>
+      <c r="E30" t="s">
+        <v>123</v>
+      </c>
+      <c r="O30" t="s">
+        <v>124</v>
+      </c>
+      <c r="X30" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" ht="12.75" customHeight="1">
+      <c r="A31" t="s">
+        <v>133</v>
+      </c>
+      <c r="B31" t="s">
+        <v>135</v>
+      </c>
+      <c r="E31" t="s">
+        <v>123</v>
+      </c>
+      <c r="O31" t="s">
+        <v>124</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" ht="12.75" customHeight="1">
+      <c r="A32" t="s">
+        <v>133</v>
+      </c>
+      <c r="B32" t="s">
+        <v>135</v>
+      </c>
+      <c r="E32" t="s">
+        <v>123</v>
+      </c>
+      <c r="O32" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="1:57" ht="12.75" customHeight="1">
+      <c r="A33" t="s">
+        <v>133</v>
+      </c>
+      <c r="B33" t="s">
+        <v>135</v>
+      </c>
+      <c r="E33" t="s">
+        <v>123</v>
+      </c>
+      <c r="O33" t="s">
+        <v>124</v>
+      </c>
+      <c r="BE33" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" spans="1:57" ht="12.75" customHeight="1">
+      <c r="A34" t="s">
+        <v>133</v>
+      </c>
+      <c r="B34" t="s">
+        <v>135</v>
+      </c>
+      <c r="E34" t="s">
+        <v>123</v>
+      </c>
+      <c r="O34" t="s">
+        <v>124</v>
+      </c>
+      <c r="AB34" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" spans="1:57" ht="12.75" customHeight="1">
+      <c r="B36" t="s">
         <v>136</v>
-      </c>
-      <c r="B20" t="s">
-        <v>138</v>
-      </c>
-      <c r="E20" t="s">
-        <v>126</v>
-      </c>
-      <c r="O20" t="s">
-        <v>127</v>
-      </c>
-      <c r="P20" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="21" spans="1:28" ht="12.75" customHeight="1">
-      <c r="A21" t="s">
-        <v>136</v>
-      </c>
-      <c r="B21" t="s">
-        <v>138</v>
-      </c>
-      <c r="E21" t="s">
-        <v>126</v>
-      </c>
-      <c r="O21" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="22" spans="1:28" ht="12.75" customHeight="1">
-      <c r="A22" t="s">
-        <v>136</v>
-      </c>
-      <c r="B22" t="s">
-        <v>138</v>
-      </c>
-      <c r="E22" t="s">
-        <v>126</v>
-      </c>
-      <c r="O22" t="s">
-        <v>127</v>
-      </c>
-      <c r="R22" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="23" spans="1:28" ht="12.75" customHeight="1">
-      <c r="A23" t="s">
-        <v>136</v>
-      </c>
-      <c r="B23" t="s">
-        <v>138</v>
-      </c>
-      <c r="E23" t="s">
-        <v>126</v>
-      </c>
-      <c r="O23" t="s">
-        <v>127</v>
-      </c>
-      <c r="S23" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="24" spans="1:28" ht="12.75" customHeight="1">
-      <c r="A24" t="s">
-        <v>136</v>
-      </c>
-      <c r="B24" t="s">
-        <v>138</v>
-      </c>
-      <c r="E24" t="s">
-        <v>126</v>
-      </c>
-      <c r="O24" t="s">
-        <v>127</v>
-      </c>
-      <c r="T24" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="25" spans="1:28" ht="12.75" customHeight="1">
-      <c r="A25" t="s">
-        <v>136</v>
-      </c>
-      <c r="B25" t="s">
-        <v>138</v>
-      </c>
-      <c r="E25" t="s">
-        <v>126</v>
-      </c>
-      <c r="O25" t="s">
-        <v>127</v>
-      </c>
-      <c r="U25" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="26" spans="1:28" ht="12.75" customHeight="1">
-      <c r="A26" t="s">
-        <v>136</v>
-      </c>
-      <c r="B26" t="s">
-        <v>138</v>
-      </c>
-      <c r="E26" t="s">
-        <v>126</v>
-      </c>
-      <c r="O26" t="s">
-        <v>127</v>
-      </c>
-      <c r="V26" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="27" spans="1:28" ht="12.75" customHeight="1">
-      <c r="A27" t="s">
-        <v>136</v>
-      </c>
-      <c r="B27" t="s">
-        <v>138</v>
-      </c>
-      <c r="E27" t="s">
-        <v>126</v>
-      </c>
-      <c r="O27" t="s">
-        <v>127</v>
-      </c>
-      <c r="W27" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="28" spans="1:28" ht="12.75" customHeight="1">
-      <c r="A28" t="s">
-        <v>136</v>
-      </c>
-      <c r="B28" t="s">
-        <v>138</v>
-      </c>
-      <c r="E28" t="s">
-        <v>126</v>
-      </c>
-      <c r="O28" t="s">
-        <v>127</v>
-      </c>
-      <c r="X28" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="29" spans="1:28" ht="12.75" customHeight="1">
-      <c r="A29" t="s">
-        <v>136</v>
-      </c>
-      <c r="B29" t="s">
-        <v>138</v>
-      </c>
-      <c r="E29" t="s">
-        <v>126</v>
-      </c>
-      <c r="O29" t="s">
-        <v>127</v>
-      </c>
-      <c r="Y29" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="30" spans="1:28" ht="12.75" customHeight="1">
-      <c r="A30" t="s">
-        <v>136</v>
-      </c>
-      <c r="B30" t="s">
-        <v>138</v>
-      </c>
-      <c r="E30" t="s">
-        <v>126</v>
-      </c>
-      <c r="O30" t="s">
-        <v>127</v>
-      </c>
-      <c r="Z30" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="31" spans="1:28" ht="12.75" customHeight="1">
-      <c r="A31" t="s">
-        <v>136</v>
-      </c>
-      <c r="B31" t="s">
-        <v>138</v>
-      </c>
-      <c r="E31" t="s">
-        <v>126</v>
-      </c>
-      <c r="O31" t="s">
-        <v>127</v>
-      </c>
-      <c r="AA31" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="32" spans="1:28" ht="12.75" customHeight="1">
-      <c r="A32" t="s">
-        <v>136</v>
-      </c>
-      <c r="B32" t="s">
-        <v>138</v>
-      </c>
-      <c r="E32" t="s">
-        <v>126</v>
-      </c>
-      <c r="O32" t="s">
-        <v>127</v>
-      </c>
-      <c r="AB32" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="33" spans="1:37" ht="12.75" customHeight="1">
-      <c r="A33" t="s">
-        <v>136</v>
-      </c>
-      <c r="B33" t="s">
-        <v>138</v>
-      </c>
-      <c r="E33" t="s">
-        <v>126</v>
-      </c>
-      <c r="O33" t="s">
-        <v>127</v>
-      </c>
-      <c r="AC33" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="34" spans="1:37" ht="12.75" customHeight="1">
-      <c r="A34" t="s">
-        <v>136</v>
-      </c>
-      <c r="B34" t="s">
-        <v>138</v>
-      </c>
-      <c r="E34" t="s">
-        <v>126</v>
-      </c>
-      <c r="O34" t="s">
-        <v>127</v>
-      </c>
-      <c r="AD34" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="36" spans="1:37" ht="12.75" customHeight="1">
-      <c r="B36" t="s">
-        <v>139</v>
       </c>
       <c r="C36">
         <v>20</v>
       </c>
-      <c r="AE36" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="38" spans="1:37" ht="12.75" customHeight="1">
+      <c r="AC36" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="38" spans="1:57" ht="12.75" customHeight="1">
       <c r="B38" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C38">
         <v>40</v>
@@ -1885,44 +1924,44 @@
         <v>70</v>
       </c>
       <c r="E38" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="40" spans="1:37" ht="12.75" customHeight="1">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="40" spans="1:57" ht="12.75" customHeight="1">
       <c r="A40" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B40" t="s">
-        <v>142</v>
-      </c>
-      <c r="AF40" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="41" spans="1:37" ht="12.75" customHeight="1">
+        <v>139</v>
+      </c>
+      <c r="AD40" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="41" spans="1:57" ht="12.75" customHeight="1">
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
     </row>
-    <row r="42" spans="1:37" ht="12.75" customHeight="1">
+    <row r="42" spans="1:57" ht="12.75" customHeight="1">
       <c r="B42" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="M42" s="3"/>
       <c r="N42" s="3"/>
-      <c r="AG42" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="43" spans="1:37" ht="12.75" customHeight="1">
+      <c r="AE42" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="43" spans="1:57" ht="12.75" customHeight="1">
       <c r="M43" s="3"/>
       <c r="N43" s="3"/>
     </row>
-    <row r="44" spans="1:37" ht="12.75" customHeight="1">
+    <row r="44" spans="1:57" ht="12.75" customHeight="1">
       <c r="A44" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B44" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C44">
         <v>55</v>
@@ -1931,15 +1970,15 @@
         <v>79</v>
       </c>
       <c r="E44" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="45" spans="1:37" ht="12.75" customHeight="1">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="45" spans="1:57" ht="12.75" customHeight="1">
       <c r="A45" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B45" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C45">
         <v>45</v>
@@ -1948,15 +1987,15 @@
         <v>79</v>
       </c>
       <c r="E45" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="47" spans="1:37" ht="12.75" customHeight="1">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="47" spans="1:57" ht="12" customHeight="1">
       <c r="A47" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B47" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C47">
         <v>21</v>
@@ -1965,41 +2004,41 @@
         <v>30</v>
       </c>
       <c r="E47" t="s">
-        <v>126</v>
-      </c>
-      <c r="AH47" t="s">
-        <v>127</v>
-      </c>
-      <c r="AI47" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="48" spans="1:37" ht="12.75" customHeight="1">
+        <v>123</v>
+      </c>
+      <c r="AF47" t="s">
+        <v>124</v>
+      </c>
+      <c r="AG47" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="48" spans="1:57" ht="12.75" customHeight="1">
       <c r="B48" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C48">
         <v>30</v>
       </c>
       <c r="E48" t="s">
-        <v>126</v>
+        <v>123</v>
+      </c>
+      <c r="AF48" t="s">
+        <v>124</v>
       </c>
       <c r="AH48" t="s">
-        <v>127</v>
-      </c>
-      <c r="AJ48" t="s">
-        <v>127</v>
-      </c>
-      <c r="AK48" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="50" spans="1:43" ht="12.75" customHeight="1">
+        <v>124</v>
+      </c>
+      <c r="AI48" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="50" spans="1:41" ht="12.75" customHeight="1">
       <c r="A50" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B50" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C50">
         <v>50</v>
@@ -2008,109 +2047,109 @@
         <v>75</v>
       </c>
     </row>
-    <row r="51" spans="1:43" ht="12.75" customHeight="1">
+    <row r="51" spans="1:41" ht="12.75" customHeight="1">
       <c r="B51" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D51">
         <v>40</v>
       </c>
-      <c r="AL51" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="53" spans="1:43" ht="12.75" customHeight="1">
+      <c r="AJ51" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="53" spans="1:41" ht="12.75" customHeight="1">
       <c r="A53" t="s">
+        <v>147</v>
+      </c>
+      <c r="B53" t="s">
+        <v>148</v>
+      </c>
+      <c r="T53" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="55" spans="1:41" ht="12.75" customHeight="1">
+      <c r="A55" t="s">
+        <v>149</v>
+      </c>
+      <c r="B55" t="s">
         <v>150</v>
       </c>
-      <c r="B53" t="s">
+    </row>
+    <row r="56" spans="1:41" ht="12.75" customHeight="1">
+      <c r="A56" t="s">
         <v>151</v>
       </c>
-      <c r="V53" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="55" spans="1:43" ht="12.75" customHeight="1">
-      <c r="A55" t="s">
+      <c r="B56" t="s">
         <v>152</v>
       </c>
-      <c r="B55" t="s">
+      <c r="E56" t="s">
+        <v>123</v>
+      </c>
+      <c r="AK56" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="57" spans="1:41" ht="12.75" customHeight="1">
+      <c r="A57" t="s">
+        <v>151</v>
+      </c>
+      <c r="B57" t="s">
+        <v>152</v>
+      </c>
+      <c r="E57" t="s">
+        <v>123</v>
+      </c>
+      <c r="AL57" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="58" spans="1:41" ht="12.75" customHeight="1">
+      <c r="A58" t="s">
+        <v>151</v>
+      </c>
+      <c r="B58" t="s">
+        <v>152</v>
+      </c>
+      <c r="E58" t="s">
+        <v>130</v>
+      </c>
+      <c r="AL58" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="59" spans="1:41" ht="12.75" customHeight="1">
+      <c r="A59" t="s">
+        <v>151</v>
+      </c>
+      <c r="B59" t="s">
+        <v>152</v>
+      </c>
+      <c r="E59" t="s">
+        <v>130</v>
+      </c>
+      <c r="AM59" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="61" spans="1:41" ht="12.75" customHeight="1">
+      <c r="A61" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="56" spans="1:43" ht="12.75" customHeight="1">
-      <c r="A56" t="s">
+      <c r="B61" t="s">
         <v>154</v>
       </c>
-      <c r="B56" t="s">
+      <c r="AN61" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="63" spans="1:41" ht="12.75" customHeight="1">
+      <c r="A63" t="s">
+        <v>153</v>
+      </c>
+      <c r="B63" t="s">
         <v>155</v>
-      </c>
-      <c r="E56" t="s">
-        <v>126</v>
-      </c>
-      <c r="AM56" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="57" spans="1:43" ht="12.75" customHeight="1">
-      <c r="A57" t="s">
-        <v>154</v>
-      </c>
-      <c r="B57" t="s">
-        <v>155</v>
-      </c>
-      <c r="E57" t="s">
-        <v>126</v>
-      </c>
-      <c r="AN57" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="58" spans="1:43" ht="12.75" customHeight="1">
-      <c r="A58" t="s">
-        <v>154</v>
-      </c>
-      <c r="B58" t="s">
-        <v>155</v>
-      </c>
-      <c r="E58" t="s">
-        <v>133</v>
-      </c>
-      <c r="AN58" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="59" spans="1:43" ht="12.75" customHeight="1">
-      <c r="A59" t="s">
-        <v>154</v>
-      </c>
-      <c r="B59" t="s">
-        <v>155</v>
-      </c>
-      <c r="E59" t="s">
-        <v>133</v>
-      </c>
-      <c r="AO59" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="61" spans="1:43" ht="12.75" customHeight="1">
-      <c r="A61" t="s">
-        <v>156</v>
-      </c>
-      <c r="B61" t="s">
-        <v>157</v>
-      </c>
-      <c r="AP61" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="63" spans="1:43" ht="12.75" customHeight="1">
-      <c r="A63" t="s">
-        <v>156</v>
-      </c>
-      <c r="B63" t="s">
-        <v>158</v>
       </c>
       <c r="C63">
         <v>50</v>
@@ -2119,26 +2158,26 @@
         <v>75</v>
       </c>
       <c r="E63" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="64" spans="1:43" ht="12.75" customHeight="1">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="64" spans="1:41" ht="12.75" customHeight="1">
       <c r="B64" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E64" t="s">
-        <v>133</v>
-      </c>
-      <c r="AQ64" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="66" spans="1:49" ht="12.75" customHeight="1">
+        <v>130</v>
+      </c>
+      <c r="AO64" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="66" spans="1:46" ht="12.75" customHeight="1">
       <c r="A66" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B66" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C66">
         <v>49</v>
@@ -2147,42 +2186,39 @@
         <v>69</v>
       </c>
     </row>
-    <row r="68" spans="1:49" ht="12.75" customHeight="1">
+    <row r="68" spans="1:46" ht="12.75" customHeight="1">
       <c r="A68" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B68" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C68">
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:49" ht="12.75" customHeight="1">
+    <row r="70" spans="1:46" ht="12.75" customHeight="1">
       <c r="B70" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H70" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="71" spans="1:49" ht="12.75" customHeight="1">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="71" spans="1:46" ht="12.75" customHeight="1">
       <c r="B71" t="s">
-        <v>163</v>
-      </c>
-      <c r="AR71" t="s">
-        <v>127</v>
-      </c>
-      <c r="AS71" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="73" spans="1:49" ht="12.75" customHeight="1">
+        <v>160</v>
+      </c>
+      <c r="AP71" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="73" spans="1:46" ht="12.75" customHeight="1">
       <c r="A73" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B73" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C73">
         <v>55</v>
@@ -2190,19 +2226,19 @@
       <c r="D73">
         <v>80</v>
       </c>
-      <c r="AT73" t="s">
-        <v>127</v>
-      </c>
-      <c r="AU73" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="75" spans="1:49" ht="12.75" customHeight="1">
+      <c r="AQ73" t="s">
+        <v>124</v>
+      </c>
+      <c r="AR73" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="75" spans="1:46" ht="12.75" customHeight="1">
       <c r="A75" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B75" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C75">
         <v>65</v>
@@ -2211,15 +2247,15 @@
         <v>75</v>
       </c>
       <c r="E75" t="s">
-        <v>133</v>
-      </c>
-      <c r="AV75" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="76" spans="1:49" ht="12.75" customHeight="1">
+        <v>130</v>
+      </c>
+      <c r="AS75" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="76" spans="1:46" ht="12.75" customHeight="1">
       <c r="B76" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C76">
         <v>65</v>
@@ -2228,341 +2264,342 @@
         <v>75</v>
       </c>
       <c r="E76" t="s">
-        <v>133</v>
-      </c>
-      <c r="AW76" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="78" spans="1:49" ht="12.75" customHeight="1">
+        <v>130</v>
+      </c>
+      <c r="AT76" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="78" spans="1:46" ht="12.75" customHeight="1">
       <c r="A78" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B78" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C78">
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:49" ht="12.75" customHeight="1">
+    <row r="80" spans="1:46" ht="12.75" customHeight="1">
       <c r="A80" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B80" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="82" spans="1:53" ht="12.75" customHeight="1">
+      <c r="A82" t="s">
+        <v>169</v>
+      </c>
+      <c r="B82" t="s">
         <v>170</v>
-      </c>
-      <c r="B80" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="82" spans="1:56" ht="12.75" customHeight="1">
-      <c r="A82" t="s">
-        <v>172</v>
-      </c>
-      <c r="B82" t="s">
-        <v>173</v>
       </c>
       <c r="D82">
         <v>34</v>
       </c>
-      <c r="AZ82" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="83" spans="1:56" ht="12.75" customHeight="1">
+      <c r="AW82" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="83" spans="1:53" ht="12.75" customHeight="1">
       <c r="B83" t="s">
-        <v>173</v>
-      </c>
-      <c r="AY83" t="s">
-        <v>127</v>
-      </c>
-      <c r="AZ83" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="85" spans="1:56" ht="12.75" customHeight="1">
+        <v>170</v>
+      </c>
+      <c r="AV83" t="s">
+        <v>124</v>
+      </c>
+      <c r="AW83" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="85" spans="1:53" ht="12.75" customHeight="1">
       <c r="A85" s="5" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B85" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D85">
         <v>26</v>
       </c>
       <c r="E85" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="86" spans="1:56" ht="12.75" customHeight="1">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="86" spans="1:53" ht="12.75" customHeight="1">
       <c r="A86" s="5" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B86" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D86">
         <v>21</v>
       </c>
       <c r="E86" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="87" spans="1:56" ht="12.75" customHeight="1">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="87" spans="1:53" ht="12.75" customHeight="1">
       <c r="A87" s="5" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B87" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D87">
         <v>26</v>
       </c>
       <c r="E87" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H87" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="89" spans="1:56" ht="12.75" customHeight="1">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="89" spans="1:53" ht="12.75" customHeight="1">
       <c r="A89" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B89" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C89">
         <v>60</v>
       </c>
     </row>
-    <row r="91" spans="1:56" ht="12.75" customHeight="1">
+    <row r="91" spans="1:53" ht="12.75" customHeight="1">
       <c r="A91" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B91" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C91">
         <v>65</v>
       </c>
     </row>
-    <row r="92" spans="1:56" ht="12.75" customHeight="1">
+    <row r="92" spans="1:53" ht="12.75" customHeight="1">
       <c r="A92" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B92" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C92">
         <v>65</v>
       </c>
-      <c r="BA92" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="93" spans="1:56" ht="12.75" customHeight="1">
+      <c r="AX92" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="93" spans="1:53" ht="12.75" customHeight="1">
       <c r="A93" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B93" t="s">
-        <v>179</v>
-      </c>
-      <c r="V93" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="94" spans="1:56" ht="12.75" customHeight="1">
+        <v>176</v>
+      </c>
+      <c r="T93" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="94" spans="1:53" ht="12.75" customHeight="1">
       <c r="A94" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B94" t="s">
-        <v>179</v>
-      </c>
-      <c r="BB94" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="95" spans="1:56" ht="12.75" customHeight="1">
+        <v>176</v>
+      </c>
+      <c r="AY94" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="95" spans="1:53" ht="12.75" customHeight="1">
       <c r="A95" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B95" t="s">
-        <v>179</v>
-      </c>
-      <c r="BC95" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="96" spans="1:56" ht="12.75" customHeight="1">
+        <v>176</v>
+      </c>
+      <c r="AZ95" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="96" spans="1:53" ht="12.75" customHeight="1">
       <c r="A96" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B96" t="s">
-        <v>179</v>
-      </c>
-      <c r="BD96" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="97" spans="1:71" ht="12.75" customHeight="1">
+        <v>176</v>
+      </c>
+      <c r="BA96" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="97" spans="1:68" ht="12.75" customHeight="1">
       <c r="A97" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B97" t="s">
-        <v>179</v>
-      </c>
-      <c r="BE97" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="98" spans="1:71" ht="12.75" customHeight="1">
+        <v>176</v>
+      </c>
+      <c r="BB97" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="98" spans="1:68" ht="12.75" customHeight="1">
       <c r="A98" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B98" t="s">
-        <v>179</v>
-      </c>
-      <c r="BF98" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="99" spans="1:71" ht="12.75" customHeight="1">
+        <v>176</v>
+      </c>
+      <c r="BC98" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="99" spans="1:68" ht="12.75" customHeight="1">
       <c r="A99" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B99" t="s">
-        <v>179</v>
-      </c>
-      <c r="BG99" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="100" spans="1:71" ht="12.75" customHeight="1">
+        <v>176</v>
+      </c>
+      <c r="BD99" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="100" spans="1:68" ht="12.75" customHeight="1">
       <c r="A100" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B100" t="s">
-        <v>179</v>
-      </c>
-      <c r="BH100" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="101" spans="1:71" ht="12.75" customHeight="1">
+        <v>176</v>
+      </c>
+      <c r="BE100" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="101" spans="1:68" ht="12.75" customHeight="1">
       <c r="A101" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B101" t="s">
-        <v>179</v>
-      </c>
-      <c r="BI101" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="102" spans="1:71" ht="12.75" customHeight="1">
+        <v>176</v>
+      </c>
+      <c r="BF101" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="102" spans="1:68" ht="12.75" customHeight="1">
       <c r="A102" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B102" t="s">
-        <v>179</v>
-      </c>
-      <c r="BJ102" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="103" spans="1:71" ht="12.75" customHeight="1">
+        <v>176</v>
+      </c>
+      <c r="BG102" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="103" spans="1:68" ht="12.75" customHeight="1">
       <c r="A103" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B103" t="s">
-        <v>179</v>
-      </c>
-      <c r="BK103" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="104" spans="1:71" ht="12.75" customHeight="1">
+        <v>176</v>
+      </c>
+      <c r="BH103" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="104" spans="1:68" ht="12.75" customHeight="1">
       <c r="A104" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B104" t="s">
-        <v>179</v>
-      </c>
-      <c r="BL104" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="105" spans="1:71" ht="12.75" customHeight="1">
+        <v>176</v>
+      </c>
+      <c r="BI104" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="105" spans="1:68" ht="12.75" customHeight="1">
       <c r="A105" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B105" t="s">
-        <v>179</v>
-      </c>
-      <c r="BM105" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="106" spans="1:71" ht="12.75" customHeight="1">
+        <v>176</v>
+      </c>
+      <c r="BJ105" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="106" spans="1:68" ht="12.75" customHeight="1">
       <c r="A106" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B106" t="s">
-        <v>179</v>
-      </c>
-      <c r="BN106" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="107" spans="1:71" ht="12.75" customHeight="1">
+        <v>176</v>
+      </c>
+      <c r="BK106" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="107" spans="1:68" ht="12.75" customHeight="1">
       <c r="A107" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B107" t="s">
-        <v>179</v>
-      </c>
-      <c r="BO107" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="108" spans="1:71" ht="12.75" customHeight="1">
+        <v>176</v>
+      </c>
+      <c r="BL107" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="108" spans="1:68" ht="12.75" customHeight="1">
       <c r="A108" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B108" t="s">
-        <v>179</v>
-      </c>
-      <c r="BP108" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="109" spans="1:71" ht="12.75" customHeight="1">
+        <v>176</v>
+      </c>
+      <c r="BM108" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="109" spans="1:68" ht="12.75" customHeight="1">
       <c r="A109" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B109" t="s">
-        <v>179</v>
-      </c>
-      <c r="BQ109" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="110" spans="1:71" ht="12.75" customHeight="1">
+        <v>176</v>
+      </c>
+      <c r="BN109" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="110" spans="1:68" ht="12.75" customHeight="1">
       <c r="A110" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B110" t="s">
-        <v>179</v>
-      </c>
-      <c r="BR110" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="112" spans="1:71" ht="12.75" customHeight="1">
+        <v>176</v>
+      </c>
+      <c r="BO110" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="111" spans="1:68" s="5" customFormat="1" ht="12.75" customHeight="1"/>
+    <row r="112" spans="1:68" ht="12.75" customHeight="1">
       <c r="A112" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B112" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C112">
         <v>19</v>
@@ -2570,16 +2607,16 @@
       <c r="D112">
         <v>64</v>
       </c>
-      <c r="BF112" t="s">
-        <v>127</v>
-      </c>
-      <c r="BS112" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="113" spans="1:72" ht="12.75" customHeight="1">
+      <c r="BC112" t="s">
+        <v>124</v>
+      </c>
+      <c r="BP112" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="113" spans="1:69" ht="12.75" customHeight="1">
       <c r="B113" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C113">
         <v>19</v>
@@ -2587,16 +2624,16 @@
       <c r="D113">
         <v>64</v>
       </c>
-      <c r="BG113" t="s">
-        <v>127</v>
-      </c>
-      <c r="BS113" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="114" spans="1:72" ht="12.75" customHeight="1">
+      <c r="BD113" t="s">
+        <v>124</v>
+      </c>
+      <c r="BP113" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="114" spans="1:69" ht="12.75" customHeight="1">
       <c r="B114" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C114">
         <v>19</v>
@@ -2604,16 +2641,16 @@
       <c r="D114">
         <v>64</v>
       </c>
-      <c r="BL114" t="s">
-        <v>127</v>
-      </c>
-      <c r="BS114" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="115" spans="1:72" ht="12.75" customHeight="1">
+      <c r="BI114" t="s">
+        <v>124</v>
+      </c>
+      <c r="BP114" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="115" spans="1:69" ht="12.75" customHeight="1">
       <c r="B115" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C115">
         <v>19</v>
@@ -2621,16 +2658,16 @@
       <c r="D115">
         <v>64</v>
       </c>
-      <c r="BM115" t="s">
-        <v>127</v>
-      </c>
-      <c r="BS115" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="116" spans="1:72" ht="12.75" customHeight="1">
+      <c r="BJ115" t="s">
+        <v>124</v>
+      </c>
+      <c r="BP115" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="116" spans="1:69" ht="12.75" customHeight="1">
       <c r="B116" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C116">
         <v>19</v>
@@ -2638,261 +2675,261 @@
       <c r="D116">
         <v>64</v>
       </c>
-      <c r="BO116" t="s">
-        <v>127</v>
-      </c>
-      <c r="BS116" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="118" spans="1:72" ht="12.75" customHeight="1">
+      <c r="BL116" t="s">
+        <v>124</v>
+      </c>
+      <c r="BP116" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="118" spans="1:69" ht="12.75" customHeight="1">
       <c r="A118" t="s">
+        <v>175</v>
+      </c>
+      <c r="B118" t="s">
         <v>178</v>
-      </c>
-      <c r="B118" t="s">
-        <v>181</v>
       </c>
       <c r="C118">
         <v>19</v>
       </c>
-      <c r="BL118" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="119" spans="1:72" ht="12.75" customHeight="1">
+      <c r="BI118" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="119" spans="1:69" ht="12.75" customHeight="1">
       <c r="B119" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C119">
         <v>19</v>
       </c>
-      <c r="BF119" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="120" spans="1:72" ht="12.75" customHeight="1">
+      <c r="BC119" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="120" spans="1:69" ht="12.75" customHeight="1">
       <c r="B120" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C120">
         <v>19</v>
       </c>
-      <c r="BG120" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="121" spans="1:72" ht="12.75" customHeight="1">
+      <c r="BD120" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="121" spans="1:69" ht="12.75" customHeight="1">
       <c r="B121" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C121">
         <v>19</v>
       </c>
-      <c r="BO121" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="122" spans="1:72" ht="12.75" customHeight="1">
+      <c r="BL121" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="122" spans="1:69" ht="12.75" customHeight="1">
       <c r="B122" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C122">
         <v>19</v>
       </c>
-      <c r="BM122" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="123" spans="1:72" ht="12.75" customHeight="1">
+      <c r="BJ122" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="123" spans="1:69" ht="12.75" customHeight="1">
       <c r="B123" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C123">
         <v>19</v>
       </c>
-      <c r="BJ123" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="124" spans="1:72" ht="12.75" customHeight="1">
+      <c r="BG123" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="124" spans="1:69" ht="12.75" customHeight="1">
       <c r="B124" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C124">
         <v>19</v>
       </c>
-      <c r="BK124" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="126" spans="1:72" ht="12.75" customHeight="1">
+      <c r="BH124" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="126" spans="1:69" ht="12.75" customHeight="1">
       <c r="A126" t="s">
+        <v>179</v>
+      </c>
+      <c r="B126" t="s">
+        <v>180</v>
+      </c>
+      <c r="BJ126" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="127" spans="1:69" ht="12.75" customHeight="1">
+      <c r="B127" t="s">
+        <v>180</v>
+      </c>
+      <c r="BL127" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="128" spans="1:69" ht="12.75" customHeight="1">
+      <c r="B128" t="s">
+        <v>180</v>
+      </c>
+      <c r="BQ128" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="129" spans="1:74" ht="12.75" customHeight="1">
+      <c r="B129" t="s">
+        <v>180</v>
+      </c>
+      <c r="BN129" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="130" spans="1:74" ht="12.75" customHeight="1">
+      <c r="B130" t="s">
+        <v>180</v>
+      </c>
+      <c r="BR130" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="132" spans="1:74" ht="12.75" customHeight="1">
+      <c r="A132" t="s">
+        <v>181</v>
+      </c>
+      <c r="B132" t="s">
         <v>182</v>
-      </c>
-      <c r="B126" t="s">
-        <v>183</v>
-      </c>
-      <c r="BM126" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="127" spans="1:72" ht="12.75" customHeight="1">
-      <c r="B127" t="s">
-        <v>183</v>
-      </c>
-      <c r="BO127" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="128" spans="1:72" ht="12.75" customHeight="1">
-      <c r="B128" t="s">
-        <v>183</v>
-      </c>
-      <c r="BT128" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="129" spans="1:77" ht="12.75" customHeight="1">
-      <c r="B129" t="s">
-        <v>183</v>
-      </c>
-      <c r="BQ129" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="130" spans="1:77" ht="12.75" customHeight="1">
-      <c r="B130" t="s">
-        <v>183</v>
-      </c>
-      <c r="BU130" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="132" spans="1:77" ht="12.75" customHeight="1">
-      <c r="A132" t="s">
-        <v>184</v>
-      </c>
-      <c r="B132" t="s">
-        <v>185</v>
       </c>
       <c r="C132">
         <v>57</v>
       </c>
     </row>
-    <row r="134" spans="1:77" ht="12.75" customHeight="1">
+    <row r="134" spans="1:74" ht="12.75" customHeight="1">
       <c r="A134" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B134" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C134">
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:77" ht="12.75" customHeight="1">
+    <row r="135" spans="1:74" ht="12.75" customHeight="1">
       <c r="B135" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E135" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H135" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="136" spans="1:77" ht="12.75" customHeight="1">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="136" spans="1:74" ht="12.75" customHeight="1">
       <c r="B136" t="s">
-        <v>188</v>
-      </c>
-      <c r="BH136" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="137" spans="1:77" ht="12.75" customHeight="1">
+        <v>185</v>
+      </c>
+      <c r="BE136" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="137" spans="1:74" ht="12.75" customHeight="1">
       <c r="B137" t="s">
-        <v>188</v>
-      </c>
-      <c r="BV137" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="138" spans="1:77" ht="12.75" customHeight="1">
+        <v>185</v>
+      </c>
+      <c r="BS137" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="138" spans="1:74" ht="12.75" customHeight="1">
       <c r="B138" t="s">
-        <v>188</v>
-      </c>
-      <c r="BW138" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="140" spans="1:77" ht="12.75" customHeight="1">
+        <v>185</v>
+      </c>
+      <c r="BT138" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="140" spans="1:74" ht="12.75" customHeight="1">
       <c r="A140" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B140" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E140" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H140" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="141" spans="1:77" ht="12.75" customHeight="1">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="141" spans="1:74" ht="12.75" customHeight="1">
       <c r="B141" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G141" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="142" spans="1:77" ht="12.75" customHeight="1">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="142" spans="1:74" ht="12.75" customHeight="1">
       <c r="B142" t="s">
-        <v>190</v>
-      </c>
-      <c r="BX142" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="143" spans="1:77" ht="12.75" customHeight="1">
+        <v>187</v>
+      </c>
+      <c r="BU142" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="143" spans="1:74" ht="12.75" customHeight="1">
       <c r="B143" t="s">
-        <v>190</v>
-      </c>
-      <c r="BY143" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="144" spans="1:77" ht="12.75" customHeight="1">
+        <v>187</v>
+      </c>
+      <c r="BV143" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="144" spans="1:74" ht="12.75" customHeight="1">
       <c r="B144" t="s">
-        <v>190</v>
-      </c>
-      <c r="BE144" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="145" spans="2:78" ht="12.75" customHeight="1">
+        <v>187</v>
+      </c>
+      <c r="BB144" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="145" spans="2:75" ht="12.75" customHeight="1">
       <c r="B145" t="s">
-        <v>190</v>
-      </c>
-      <c r="BZ145" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="146" spans="2:78" ht="12.75" customHeight="1">
+        <v>187</v>
+      </c>
+      <c r="BW145" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="146" spans="2:75" ht="12.75" customHeight="1">
       <c r="B146" t="s">
-        <v>190</v>
-      </c>
-      <c r="BQ146" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="147" spans="2:78" ht="12.75" customHeight="1">
+        <v>187</v>
+      </c>
+      <c r="BN146" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="147" spans="2:75" ht="12.75" customHeight="1">
       <c r="B147" t="s">
-        <v>190</v>
-      </c>
-      <c r="BH147" t="s">
-        <v>127</v>
+        <v>187</v>
+      </c>
+      <c r="BE147" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Check in the NaN tests
</commit_message>
<xml_diff>
--- a/Preventive Care Screening MedStart.xlsx
+++ b/Preventive Care Screening MedStart.xlsx
@@ -1240,7 +1240,7 @@
   <dimension ref="A1:BX147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A147" sqref="A3:BX147"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1672,7 +1672,7 @@
         <v>198</v>
       </c>
       <c r="D4">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <v>24</v>

</xml_diff>

<commit_message>
Added tooltip that explains the particular decision. Shows row number (in spreadsheet) for the rule, plus the column name and value
</commit_message>
<xml_diff>
--- a/Preventive Care Screening MedStart.xlsx
+++ b/Preventive Care Screening MedStart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="2760" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
+    <workbookView xWindow="1040" yWindow="5240" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -772,8 +772,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="57">
+  <cellStyleXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -851,7 +861,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="57">
+  <cellStyles count="67">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -880,6 +890,11 @@
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -908,6 +923,11 @@
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1240,7 +1260,10 @@
   <dimension ref="A1:BX147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="AF20" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="AM3" sqref="AM3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>

</xml_diff>